<commit_message>
spring batch - row count corrected
</commit_message>
<xml_diff>
--- a/springwebapp/src/main/resources/userdetails.xlsx
+++ b/springwebapp/src/main/resources/userdetails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse workspaces\workouts\springbatch\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workouts\git\workouts\springwebapp\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9F6F665-BD39-4155-9FEB-F358BBCF3631}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB20BC8-FEC9-49B0-9909-66A694E45DC4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{8499759C-235A-459C-B680-0CA812F880C5}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>vinoth</t>
   </si>
   <si>
     <t>vimal</t>
+  </si>
+  <si>
+    <t>sridhar</t>
+  </si>
+  <si>
+    <t>vijaya</t>
   </si>
 </sst>
 </file>
@@ -382,34 +388,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206D16C3-D465-4711-9502-2E012C78E6B6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>28</v>
+      <c r="B2">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>26</v>
+      <c r="B3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>